<commit_message>
Started looking at graphics for my blog post
</commit_message>
<xml_diff>
--- a/DepthCharges/AirborneDroppedMines.xlsx
+++ b/DepthCharges/AirborneDroppedMines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26505"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\DepthCharges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD548C4E-D9D1-4795-88F5-549DD297DF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA12FA4-48DD-4192-B123-50EC35817E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-    <pivotCache cacheId="3" r:id="rId4"/>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -415,152 +415,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0A2FE024-92FE-43A0-9713-6851D4004EF1}"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <fill>
@@ -782,16 +642,16 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
     <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{7C354013-5777-434E-AE4C-CFEE7785F191}">
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="totalRow" dxfId="48"/>
-      <tableStyleElement type="firstColumn" dxfId="47"/>
-      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="totalRow" dxfId="28"/>
+      <tableStyleElement type="firstColumn" dxfId="27"/>
+      <tableStyleElement type="firstRowStripe" dxfId="26"/>
     </tableStyle>
     <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{0F62376E-C7C2-4D0A-80AF-3486931EC7A3}">
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="totalRow" dxfId="44"/>
-      <tableStyleElement type="firstColumn" dxfId="43"/>
-      <tableStyleElement type="firstRowStripe" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="totalRow" dxfId="24"/>
+      <tableStyleElement type="firstColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
     </tableStyle>
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{D5A5F521-9AF8-494D-A293-CE4730E89140}"/>
   </tableStyles>
@@ -804,6 +664,1214 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[AirborneDroppedMines.xlsx]Raw_Airborn!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Raw_Airborn!$U$62:$U$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Airborne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Raw_Airborn!$S$64:$T$70</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1945</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Raw_Airborn!$U$64:$U$70</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18392</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CB2-403E-B8A9-ED60DE0A3FA7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Raw_Airborn!$V$62:$V$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SUBMARINE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Raw_Airborn!$S$64:$T$70</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1945</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Raw_Airborn!$V$64:$V$70</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0CB2-403E-B8A9-ED60DE0A3FA7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Raw_Airborn!$W$62:$W$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SURFACE CRAFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Raw_Airborn!$S$64:$T$70</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1945</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Raw_Airborn!$W$64:$W$70</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4116</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0CB2-403E-B8A9-ED60DE0A3FA7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1375634672"/>
+        <c:axId val="1375631792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1375634672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1375631792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1375631792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1375634672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -950,6 +2018,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1103244</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>109330</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16990C1A-1CBB-CE07-47B9-BA8D349A6FC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3561,7 +4665,406 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03D75A69-9385-4459-86C0-8514CBC7C464}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1D70F20-72AF-44B2-9D42-31DAC2A09F92}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="S62:X70" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1">
+      <items count="7">
+        <item x="0" e="0"/>
+        <item x="1" e="0"/>
+        <item x="2" e="0"/>
+        <item x="3" e="0"/>
+        <item x="4" e="0"/>
+        <item x="5" e="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Value" fld="3" baseField="1" baseItem="0" numFmtId="3"/>
+  </dataFields>
+  <formats count="21">
+    <format dxfId="21">
+      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="4" selected="0">
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="2" selected="0">
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="21">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="2">
+    <rowHierarchyUsage hierarchyUsage="11"/>
+    <rowHierarchyUsage hierarchyUsage="13"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="8"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings>
+        <x15:activeTabTopLevelEntity name="[Combined]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03D75A69-9385-4459-86C0-8514CBC7C464}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="T44:AA53" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1">
@@ -3697,369 +5200,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1D70F20-72AF-44B2-9D42-31DAC2A09F92}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="S62:X70" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
-  <pivotFields count="4">
-    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1">
-      <items count="7">
-        <item x="0" e="0"/>
-        <item x="1" e="0"/>
-        <item x="2" e="0"/>
-        <item x="3" e="0"/>
-        <item x="4" e="0"/>
-        <item x="5" e="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Value" fld="3" baseField="1" baseItem="0" numFmtId="3"/>
-  </dataFields>
-  <formats count="21">
-    <format dxfId="41">
-      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
-      <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="39">
-      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="2" selected="0">
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="2" selected="0">
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea field="1" grandCol="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="4" selected="0">
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="2" selected="0">
-            <x v="2"/>
-            <x v="3"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea field="2" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotHierarchies count="21">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="2">
-    <rowHierarchyUsage hierarchyUsage="11"/>
-    <rowHierarchyUsage hierarchyUsage="13"/>
-  </rowHierarchiesUsage>
-  <colHierarchiesUsage count="1">
-    <colHierarchyUsage hierarchyUsage="8"/>
-  </colHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings>
-        <x15:activeTabTopLevelEntity name="[Combined]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD6E8CFA-8D2D-4D79-BEAF-267C21F2A4AB}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD6E8CFA-8D2D-4D79-BEAF-267C21F2A4AB}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="F1:J9" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField compact="0" outline="0" showAll="0">
@@ -4261,7 +5403,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{394EF55B-5601-416F-89B0-8FC05269FBDE}" name="Table4" displayName="Table4" ref="A1:D373" totalsRowShown="0">
   <autoFilter ref="A1:D373" xr:uid="{394EF55B-5601-416F-89B0-8FC05269FBDE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E8AD9C6E-7FFA-4802-BD20-C77E40991A77}" name="Date" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{E8AD9C6E-7FFA-4802-BD20-C77E40991A77}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E64A40D9-8354-4A2B-AAE9-B4FAC7A5A3F8}" name="Type"/>
     <tableColumn id="3" xr3:uid="{CB38B31A-A814-4CB4-B2D9-360A348E8533}" name="Mark"/>
     <tableColumn id="4" xr3:uid="{62CA5B75-415C-4054-BF6A-A5302E7218A9}" name="Value"/>
@@ -4594,12 +5736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="9924" ySplit="3960" topLeftCell="R62" activePane="bottomRight"/>
-      <selection activeCell="N34" sqref="N34"/>
-      <selection pane="topRight" activeCell="X52" sqref="X52"/>
-      <selection pane="bottomLeft" activeCell="O64" sqref="O64"/>
-      <selection pane="bottomRight" activeCell="R67" sqref="R67"/>
+    <sheetView tabSelected="1" topLeftCell="P67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W72" sqref="W72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>